<commit_message>
Fixed weighting for ccpi data
</commit_message>
<xml_diff>
--- a/Current_Model_Build.xlsx
+++ b/Current_Model_Build.xlsx
@@ -546,16 +546,16 @@
         <v>6.848648648648648</v>
       </c>
       <c r="H3" t="n">
-        <v>24.43</v>
+        <v>61.075</v>
       </c>
       <c r="I3" t="n">
-        <v>8.92</v>
+        <v>44.6</v>
       </c>
       <c r="J3" t="n">
-        <v>10.95</v>
+        <v>54.74999999999999</v>
       </c>
       <c r="K3" t="n">
-        <v>13.87</v>
+        <v>69.34999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -581,16 +581,16 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>24.92</v>
+        <v>62.3</v>
       </c>
       <c r="I4" t="n">
-        <v>3.24</v>
+        <v>16.2</v>
       </c>
       <c r="J4" t="n">
-        <v>13.78</v>
+        <v>68.89999999999999</v>
       </c>
       <c r="K4" t="n">
-        <v>4.86</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="5">
@@ -622,16 +622,16 @@
         <v>6.62037037037037</v>
       </c>
       <c r="H5" t="n">
-        <v>25.29</v>
+        <v>63.225</v>
       </c>
       <c r="I5" t="n">
-        <v>6.26</v>
+        <v>31.3</v>
       </c>
       <c r="J5" t="n">
-        <v>10.55</v>
+        <v>52.75</v>
       </c>
       <c r="K5" t="n">
-        <v>12.9</v>
+        <v>64.5</v>
       </c>
     </row>
     <row r="6">
@@ -686,16 +686,16 @@
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>20.83</v>
+        <v>52.075</v>
       </c>
       <c r="I7" t="n">
-        <v>8.960000000000001</v>
+        <v>44.8</v>
       </c>
       <c r="J7" t="n">
-        <v>12.04</v>
+        <v>60.2</v>
       </c>
       <c r="K7" t="n">
-        <v>5.11</v>
+        <v>25.55</v>
       </c>
     </row>
     <row r="8">
@@ -723,16 +723,16 @@
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>21.67</v>
+        <v>54.175</v>
       </c>
       <c r="I8" t="n">
-        <v>11.63</v>
+        <v>58.15</v>
       </c>
       <c r="J8" t="n">
-        <v>12.64</v>
+        <v>63.2</v>
       </c>
       <c r="K8" t="n">
-        <v>11.38</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="9">
@@ -760,16 +760,16 @@
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>22.9</v>
+        <v>57.24999999999999</v>
       </c>
       <c r="I9" t="n">
-        <v>7.64</v>
+        <v>38.2</v>
       </c>
       <c r="J9" t="n">
-        <v>15.3</v>
+        <v>76.5</v>
       </c>
       <c r="K9" t="n">
-        <v>7.26</v>
+        <v>36.3</v>
       </c>
     </row>
     <row r="10">
@@ -828,16 +828,16 @@
         <v>7.920754716981132</v>
       </c>
       <c r="H11" t="n">
-        <v>29.8</v>
+        <v>74.5</v>
       </c>
       <c r="I11" t="n">
-        <v>15.01</v>
+        <v>75.05</v>
       </c>
       <c r="J11" t="n">
-        <v>13.53</v>
+        <v>67.64999999999999</v>
       </c>
       <c r="K11" t="n">
-        <v>17.24</v>
+        <v>86.19999999999999</v>
       </c>
     </row>
     <row r="12">
@@ -865,16 +865,16 @@
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
-        <v>27.35</v>
+        <v>68.375</v>
       </c>
       <c r="I12" t="n">
-        <v>12.67</v>
+        <v>63.35</v>
       </c>
       <c r="J12" t="n">
-        <v>15.31</v>
+        <v>76.55</v>
       </c>
       <c r="K12" t="n">
-        <v>16.74</v>
+        <v>83.69999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -906,16 +906,16 @@
         <v>7.712000000000001</v>
       </c>
       <c r="H13" t="n">
-        <v>25.38</v>
+        <v>63.45</v>
       </c>
       <c r="I13" t="n">
-        <v>13.39</v>
+        <v>66.95</v>
       </c>
       <c r="J13" t="n">
-        <v>4.49</v>
+        <v>22.45</v>
       </c>
       <c r="K13" t="n">
-        <v>17.86</v>
+        <v>89.3</v>
       </c>
     </row>
     <row r="14">
@@ -947,16 +947,16 @@
         <v>6.725000000000001</v>
       </c>
       <c r="H14" t="n">
-        <v>27.02</v>
+        <v>67.55</v>
       </c>
       <c r="I14" t="n">
-        <v>4.55</v>
+        <v>22.75</v>
       </c>
       <c r="J14" t="n">
-        <v>12.84</v>
+        <v>64.19999999999999</v>
       </c>
       <c r="K14" t="n">
-        <v>12.71</v>
+        <v>63.55</v>
       </c>
     </row>
     <row r="15">
@@ -988,16 +988,16 @@
         <v>6.719617224880383</v>
       </c>
       <c r="H15" t="n">
-        <v>28.47</v>
+        <v>71.175</v>
       </c>
       <c r="I15" t="n">
-        <v>7.38</v>
+        <v>36.9</v>
       </c>
       <c r="J15" t="n">
-        <v>14.54</v>
+        <v>72.69999999999999</v>
       </c>
       <c r="K15" t="n">
-        <v>15.39</v>
+        <v>76.95</v>
       </c>
     </row>
     <row r="16">
@@ -1029,16 +1029,16 @@
         <v>6.304761904761905</v>
       </c>
       <c r="H16" t="n">
-        <v>25.73</v>
+        <v>64.325</v>
       </c>
       <c r="I16" t="n">
-        <v>7.92</v>
+        <v>39.6</v>
       </c>
       <c r="J16" t="n">
-        <v>16.24</v>
+        <v>81.19999999999999</v>
       </c>
       <c r="K16" t="n">
-        <v>10.45</v>
+        <v>52.24999999999999</v>
       </c>
     </row>
     <row r="17">
@@ -1066,16 +1066,16 @@
       </c>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
-        <v>24.3</v>
+        <v>60.75</v>
       </c>
       <c r="I17" t="n">
-        <v>6.17</v>
+        <v>30.85</v>
       </c>
       <c r="J17" t="n">
-        <v>12.9</v>
+        <v>64.5</v>
       </c>
       <c r="K17" t="n">
-        <v>2.56</v>
+        <v>12.8</v>
       </c>
     </row>
     <row r="18">
@@ -1136,16 +1136,16 @@
         <v>7.559615384615385</v>
       </c>
       <c r="H19" t="n">
-        <v>20.17</v>
+        <v>50.425</v>
       </c>
       <c r="I19" t="n">
-        <v>7.06</v>
+        <v>35.3</v>
       </c>
       <c r="J19" t="n">
-        <v>14.11</v>
+        <v>70.55</v>
       </c>
       <c r="K19" t="n">
-        <v>10.08</v>
+        <v>50.4</v>
       </c>
     </row>
     <row r="20">
@@ -1177,16 +1177,16 @@
         <v>6.626086956521739</v>
       </c>
       <c r="H20" t="n">
-        <v>23.2</v>
+        <v>57.99999999999999</v>
       </c>
       <c r="I20" t="n">
-        <v>7.38</v>
+        <v>36.9</v>
       </c>
       <c r="J20" t="n">
-        <v>13.52</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="K20" t="n">
-        <v>6.49</v>
+        <v>32.45</v>
       </c>
     </row>
     <row r="21">
@@ -1272,16 +1272,16 @@
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="n">
-        <v>20.52</v>
+        <v>51.3</v>
       </c>
       <c r="I23" t="n">
-        <v>12.63</v>
+        <v>63.15</v>
       </c>
       <c r="J23" t="n">
-        <v>13.15</v>
+        <v>65.75</v>
       </c>
       <c r="K23" t="n">
-        <v>11.38</v>
+        <v>56.9</v>
       </c>
     </row>
     <row r="24">
@@ -1307,16 +1307,16 @@
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="n">
-        <v>27.23</v>
+        <v>68.075</v>
       </c>
       <c r="I24" t="n">
-        <v>9.949999999999999</v>
+        <v>49.74999999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>14.08</v>
+        <v>70.39999999999999</v>
       </c>
       <c r="K24" t="n">
-        <v>11.73</v>
+        <v>58.65</v>
       </c>
     </row>
     <row r="25">
@@ -1348,16 +1348,16 @@
         <v>6.143243243243243</v>
       </c>
       <c r="H25" t="n">
-        <v>32.23</v>
+        <v>80.57499999999999</v>
       </c>
       <c r="I25" t="n">
-        <v>9.5</v>
+        <v>47.5</v>
       </c>
       <c r="J25" t="n">
-        <v>11.84</v>
+        <v>59.2</v>
       </c>
       <c r="K25" t="n">
-        <v>11.52</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="26">
@@ -1383,16 +1383,16 @@
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="n">
-        <v>28.39</v>
+        <v>70.97499999999999</v>
       </c>
       <c r="I26" t="n">
-        <v>6.93</v>
+        <v>34.65</v>
       </c>
       <c r="J26" t="n">
-        <v>15.64</v>
+        <v>78.2</v>
       </c>
       <c r="K26" t="n">
-        <v>8.85</v>
+        <v>44.24999999999999</v>
       </c>
     </row>
     <row r="27">
@@ -1478,16 +1478,16 @@
         <v>7.371428571428572</v>
       </c>
       <c r="H29" t="n">
-        <v>27.24</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="I29" t="n">
-        <v>10.59</v>
+        <v>52.95</v>
       </c>
       <c r="J29" t="n">
-        <v>13.48</v>
+        <v>67.39999999999999</v>
       </c>
       <c r="K29" t="n">
-        <v>18.67</v>
+        <v>93.34999999999999</v>
       </c>
     </row>
     <row r="30">
@@ -1546,16 +1546,16 @@
         <v>7.705970149253731</v>
       </c>
       <c r="H31" t="n">
-        <v>29.45</v>
+        <v>73.625</v>
       </c>
       <c r="I31" t="n">
-        <v>19.12</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="J31" t="n">
-        <v>8.960000000000001</v>
+        <v>44.8</v>
       </c>
       <c r="K31" t="n">
-        <v>9.949999999999999</v>
+        <v>49.74999999999999</v>
       </c>
     </row>
     <row r="32">
@@ -1587,16 +1587,16 @@
         <v>6.43235294117647</v>
       </c>
       <c r="H32" t="n">
-        <v>20.51</v>
+        <v>51.275</v>
       </c>
       <c r="I32" t="n">
-        <v>5.79</v>
+        <v>28.95</v>
       </c>
       <c r="J32" t="n">
-        <v>11.78</v>
+        <v>58.89999999999999</v>
       </c>
       <c r="K32" t="n">
-        <v>6.33</v>
+        <v>31.65</v>
       </c>
     </row>
     <row r="33">
@@ -1628,16 +1628,16 @@
         <v>6.615</v>
       </c>
       <c r="H33" t="n">
-        <v>29.78</v>
+        <v>74.45</v>
       </c>
       <c r="I33" t="n">
-        <v>8.779999999999999</v>
+        <v>43.89999999999999</v>
       </c>
       <c r="J33" t="n">
-        <v>15.59</v>
+        <v>77.94999999999999</v>
       </c>
       <c r="K33" t="n">
-        <v>13.24</v>
+        <v>66.2</v>
       </c>
     </row>
     <row r="34">
@@ -1665,16 +1665,16 @@
       </c>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
-        <v>29.94</v>
+        <v>74.84999999999999</v>
       </c>
       <c r="I34" t="n">
-        <v>5.01</v>
+        <v>25.05</v>
       </c>
       <c r="J34" t="n">
-        <v>14.77</v>
+        <v>73.84999999999999</v>
       </c>
       <c r="K34" t="n">
-        <v>11.78</v>
+        <v>58.89999999999999</v>
       </c>
     </row>
     <row r="35">
@@ -1702,16 +1702,16 @@
       </c>
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
-        <v>18.85</v>
+        <v>47.125</v>
       </c>
       <c r="I35" t="n">
-        <v>2.26</v>
+        <v>11.3</v>
       </c>
       <c r="J35" t="n">
-        <v>8.43</v>
+        <v>42.15</v>
       </c>
       <c r="K35" t="n">
-        <v>1.45</v>
+        <v>7.249999999999999</v>
       </c>
     </row>
     <row r="36">
@@ -1793,16 +1793,16 @@
       </c>
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
-        <v>23.37</v>
+        <v>58.425</v>
       </c>
       <c r="I38" t="n">
-        <v>7.21</v>
+        <v>36.05</v>
       </c>
       <c r="J38" t="n">
-        <v>12.35</v>
+        <v>61.74999999999999</v>
       </c>
       <c r="K38" t="n">
-        <v>10.64</v>
+        <v>53.2</v>
       </c>
     </row>
     <row r="39">
@@ -1834,16 +1834,16 @@
         <v>6.825925925925926</v>
       </c>
       <c r="H39" t="n">
-        <v>27.78</v>
+        <v>69.45</v>
       </c>
       <c r="I39" t="n">
-        <v>6.97</v>
+        <v>34.84999999999999</v>
       </c>
       <c r="J39" t="n">
-        <v>14.68</v>
+        <v>73.39999999999999</v>
       </c>
       <c r="K39" t="n">
-        <v>13.94</v>
+        <v>69.69999999999999</v>
       </c>
     </row>
     <row r="40">
@@ -1875,16 +1875,16 @@
         <v>7.205217391304348</v>
       </c>
       <c r="H40" t="n">
-        <v>32.93</v>
+        <v>82.32499999999999</v>
       </c>
       <c r="I40" t="n">
-        <v>15.23</v>
+        <v>76.14999999999999</v>
       </c>
       <c r="J40" t="n">
-        <v>10.42</v>
+        <v>52.1</v>
       </c>
       <c r="K40" t="n">
-        <v>10.8</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41">
@@ -1916,16 +1916,16 @@
         <v>7.320245398773007</v>
       </c>
       <c r="H41" t="n">
-        <v>27.77</v>
+        <v>69.425</v>
       </c>
       <c r="I41" t="n">
-        <v>7.63</v>
+        <v>38.15</v>
       </c>
       <c r="J41" t="n">
-        <v>15.03</v>
+        <v>75.14999999999999</v>
       </c>
       <c r="K41" t="n">
-        <v>11.52</v>
+        <v>57.6</v>
       </c>
     </row>
     <row r="42">
@@ -1984,16 +1984,16 @@
         <v>7.831083481349911</v>
       </c>
       <c r="H43" t="n">
-        <v>30.95</v>
+        <v>77.375</v>
       </c>
       <c r="I43" t="n">
-        <v>5.2</v>
+        <v>26</v>
       </c>
       <c r="J43" t="n">
-        <v>16.63</v>
+        <v>83.14999999999999</v>
       </c>
       <c r="K43" t="n">
-        <v>9.58</v>
+        <v>47.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exported climate risk as its own added it to current model build excel file
</commit_message>
<xml_diff>
--- a/Current_Model_Build.xlsx
+++ b/Current_Model_Build.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Poplation</t>
+          <t>Population</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -487,6 +487,36 @@
       <c r="K1" s="1" t="inlineStr">
         <is>
           <t>2024_CCPI_Climate_Policy</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>2023_WPR_ND_Risk_Exposure</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>2023_WPR_ND_Risk_Vulnerability</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>2023_WPR_ND_Risk_Susceptibility</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>2023_WPR_ND_Lack_Adaptive_Capacities</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>2023_WPR_ND_Lack_Coping_Capacities</t>
         </is>
       </c>
     </row>
@@ -516,6 +546,24 @@
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="N2" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="O2" t="n">
+        <v>11.51</v>
+      </c>
+      <c r="P2" t="n">
+        <v>37.51</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>11.28</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -556,6 +604,24 @@
       </c>
       <c r="K3" t="n">
         <v>69.34999999999999</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N3" t="n">
+        <v>8.84</v>
+      </c>
+      <c r="O3" t="n">
+        <v>4.44</v>
+      </c>
+      <c r="P3" t="n">
+        <v>19.53</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>7.98</v>
       </c>
     </row>
     <row r="4">
@@ -592,6 +658,24 @@
       <c r="K4" t="n">
         <v>24.3</v>
       </c>
+      <c r="L4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="N4" t="n">
+        <v>11.14</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="P4" t="n">
+        <v>36.57</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>5.83</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -632,6 +716,24 @@
       </c>
       <c r="K5" t="n">
         <v>64.5</v>
+      </c>
+      <c r="L5" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="N5" t="n">
+        <v>18.49</v>
+      </c>
+      <c r="O5" t="n">
+        <v>8.029999999999999</v>
+      </c>
+      <c r="P5" t="n">
+        <v>28.91</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>27.21</v>
       </c>
     </row>
     <row r="6">
@@ -660,6 +762,24 @@
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="N6" t="n">
+        <v>20.28</v>
+      </c>
+      <c r="O6" t="n">
+        <v>14.13</v>
+      </c>
+      <c r="P6" t="n">
+        <v>51.26</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>11.51</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -697,6 +817,24 @@
       <c r="K7" t="n">
         <v>25.55</v>
       </c>
+      <c r="L7" t="n">
+        <v>5</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N7" t="n">
+        <v>19.15</v>
+      </c>
+      <c r="O7" t="n">
+        <v>17.48</v>
+      </c>
+      <c r="P7" t="n">
+        <v>46.46</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>8.65</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -734,6 +872,24 @@
       <c r="K8" t="n">
         <v>56.9</v>
       </c>
+      <c r="L8" t="n">
+        <v>6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="N8" t="n">
+        <v>14.48</v>
+      </c>
+      <c r="O8" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="P8" t="n">
+        <v>37.03</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>9.6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -770,6 +926,24 @@
       </c>
       <c r="K9" t="n">
         <v>36.3</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="N9" t="n">
+        <v>12.43</v>
+      </c>
+      <c r="O9" t="n">
+        <v>7.26</v>
+      </c>
+      <c r="P9" t="n">
+        <v>35.48</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>7.45</v>
       </c>
     </row>
     <row r="10">
@@ -798,6 +972,14 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>8</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -838,6 +1020,24 @@
       </c>
       <c r="K11" t="n">
         <v>86.19999999999999</v>
+      </c>
+      <c r="L11" t="n">
+        <v>9</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="N11" t="n">
+        <v>5.42</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="P11" t="n">
+        <v>28.66</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1.6</v>
       </c>
     </row>
     <row r="12">
@@ -876,6 +1076,24 @@
       <c r="K12" t="n">
         <v>83.69999999999999</v>
       </c>
+      <c r="L12" t="n">
+        <v>10</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="N12" t="n">
+        <v>7.87</v>
+      </c>
+      <c r="O12" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="P12" t="n">
+        <v>37.87</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>1.92</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -917,6 +1135,24 @@
       <c r="K13" t="n">
         <v>89.3</v>
       </c>
+      <c r="L13" t="n">
+        <v>11</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="N13" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="O13" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="P13" t="n">
+        <v>26.53</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.49</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -958,6 +1194,24 @@
       <c r="K14" t="n">
         <v>63.55</v>
       </c>
+      <c r="L14" t="n">
+        <v>12</v>
+      </c>
+      <c r="M14" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="N14" t="n">
+        <v>20.23</v>
+      </c>
+      <c r="O14" t="n">
+        <v>8.460000000000001</v>
+      </c>
+      <c r="P14" t="n">
+        <v>33.29</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>29.38</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -999,6 +1253,24 @@
       <c r="K15" t="n">
         <v>76.95</v>
       </c>
+      <c r="L15" t="n">
+        <v>13</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="N15" t="n">
+        <v>9.279999999999999</v>
+      </c>
+      <c r="O15" t="n">
+        <v>7.02</v>
+      </c>
+      <c r="P15" t="n">
+        <v>35.42</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>3.21</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1039,6 +1311,24 @@
       </c>
       <c r="K16" t="n">
         <v>52.24999999999999</v>
+      </c>
+      <c r="L16" t="n">
+        <v>14</v>
+      </c>
+      <c r="M16" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="N16" t="n">
+        <v>8.93</v>
+      </c>
+      <c r="O16" t="n">
+        <v>8.82</v>
+      </c>
+      <c r="P16" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>8.09</v>
       </c>
     </row>
     <row r="17">
@@ -1076,6 +1366,24 @@
       </c>
       <c r="K17" t="n">
         <v>12.8</v>
+      </c>
+      <c r="L17" t="n">
+        <v>15</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="N17" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="O17" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="P17" t="n">
+        <v>10.36</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>9.220000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -1106,6 +1414,24 @@
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
+      <c r="L18" t="n">
+        <v>16</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="N18" t="n">
+        <v>5.97</v>
+      </c>
+      <c r="O18" t="n">
+        <v>6.26</v>
+      </c>
+      <c r="P18" t="n">
+        <v>19.86</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>1.71</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1147,6 +1473,24 @@
       <c r="K19" t="n">
         <v>50.4</v>
       </c>
+      <c r="L19" t="n">
+        <v>17</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="N19" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="O19" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="P19" t="n">
+        <v>24.76</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>3.43</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1187,6 +1531,24 @@
       </c>
       <c r="K20" t="n">
         <v>32.45</v>
+      </c>
+      <c r="L20" t="n">
+        <v>18</v>
+      </c>
+      <c r="M20" t="n">
+        <v>8.69</v>
+      </c>
+      <c r="N20" t="n">
+        <v>11.43</v>
+      </c>
+      <c r="O20" t="n">
+        <v>7.96</v>
+      </c>
+      <c r="P20" t="n">
+        <v>35.77</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>5.25</v>
       </c>
     </row>
     <row r="21">
@@ -1221,6 +1583,14 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
+      <c r="L21" t="n">
+        <v>19</v>
+      </c>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1248,6 +1618,14 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
+      <c r="L22" t="n">
+        <v>20</v>
+      </c>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1283,6 +1661,24 @@
       <c r="K23" t="n">
         <v>56.9</v>
       </c>
+      <c r="L23" t="n">
+        <v>21</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="N23" t="n">
+        <v>9.49</v>
+      </c>
+      <c r="O23" t="n">
+        <v>9.289999999999999</v>
+      </c>
+      <c r="P23" t="n">
+        <v>40.13</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>2.29</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1318,6 +1714,24 @@
       <c r="K24" t="n">
         <v>58.65</v>
       </c>
+      <c r="L24" t="n">
+        <v>22</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="N24" t="n">
+        <v>66.43000000000001</v>
+      </c>
+      <c r="O24" t="n">
+        <v>61.03</v>
+      </c>
+      <c r="P24" t="n">
+        <v>68.44</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>70.18000000000001</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1358,6 +1772,24 @@
       </c>
       <c r="K25" t="n">
         <v>57.6</v>
+      </c>
+      <c r="L25" t="n">
+        <v>23</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="N25" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="O25" t="n">
+        <v>5.36</v>
+      </c>
+      <c r="P25" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>5.76</v>
       </c>
     </row>
     <row r="26">
@@ -1393,6 +1825,24 @@
       </c>
       <c r="K26" t="n">
         <v>44.24999999999999</v>
+      </c>
+      <c r="L26" t="n">
+        <v>24</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="N26" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="O26" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="P26" t="n">
+        <v>13.99</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>2.07</v>
       </c>
     </row>
     <row r="27">
@@ -1421,6 +1871,24 @@
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
+      <c r="L27" t="n">
+        <v>25</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N27" t="n">
+        <v>17.72</v>
+      </c>
+      <c r="O27" t="n">
+        <v>11.78</v>
+      </c>
+      <c r="P27" t="n">
+        <v>48.54</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>9.73</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1448,6 +1916,24 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" t="n">
+        <v>26</v>
+      </c>
+      <c r="M28" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="N28" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="O28" t="n">
+        <v>8.369999999999999</v>
+      </c>
+      <c r="P28" t="n">
+        <v>44.66</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>4.39</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1488,6 +1974,24 @@
       </c>
       <c r="K29" t="n">
         <v>93.34999999999999</v>
+      </c>
+      <c r="L29" t="n">
+        <v>27</v>
+      </c>
+      <c r="M29" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="N29" t="n">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="O29" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="P29" t="n">
+        <v>33.07</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>3.28</v>
       </c>
     </row>
     <row r="30">
@@ -1516,6 +2020,24 @@
       <c r="I30" t="inlineStr"/>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
+      <c r="L30" t="n">
+        <v>28</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="N30" t="n">
+        <v>5.12</v>
+      </c>
+      <c r="O30" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="P30" t="n">
+        <v>7.43</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>2.24</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1557,6 +2079,24 @@
       <c r="K31" t="n">
         <v>49.74999999999999</v>
       </c>
+      <c r="L31" t="n">
+        <v>29</v>
+      </c>
+      <c r="M31" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="N31" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="O31" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="P31" t="n">
+        <v>23.67</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>3.18</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1598,6 +2138,24 @@
       <c r="K32" t="n">
         <v>31.65</v>
       </c>
+      <c r="L32" t="n">
+        <v>30</v>
+      </c>
+      <c r="M32" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="N32" t="n">
+        <v>10.28</v>
+      </c>
+      <c r="O32" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="P32" t="n">
+        <v>40.15</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>5.21</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1638,6 +2196,24 @@
       </c>
       <c r="K33" t="n">
         <v>66.2</v>
+      </c>
+      <c r="L33" t="n">
+        <v>31</v>
+      </c>
+      <c r="M33" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="N33" t="n">
+        <v>25.96</v>
+      </c>
+      <c r="O33" t="n">
+        <v>18.99</v>
+      </c>
+      <c r="P33" t="n">
+        <v>67.72</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>13.61</v>
       </c>
     </row>
     <row r="34">
@@ -1676,6 +2252,24 @@
       <c r="K34" t="n">
         <v>58.89999999999999</v>
       </c>
+      <c r="L34" t="n">
+        <v>32</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="N34" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="O34" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="P34" t="n">
+        <v>47.28</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>8.68</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1712,6 +2306,24 @@
       </c>
       <c r="K35" t="n">
         <v>7.249999999999999</v>
+      </c>
+      <c r="L35" t="n">
+        <v>33</v>
+      </c>
+      <c r="M35" t="n">
+        <v>28.35</v>
+      </c>
+      <c r="N35" t="n">
+        <v>28.05</v>
+      </c>
+      <c r="O35" t="n">
+        <v>14.97</v>
+      </c>
+      <c r="P35" t="n">
+        <v>37.81</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>39</v>
       </c>
     </row>
     <row r="36">
@@ -1740,6 +2352,24 @@
       <c r="I36" t="inlineStr"/>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
+      <c r="L36" t="n">
+        <v>34</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="N36" t="n">
+        <v>17.92</v>
+      </c>
+      <c r="O36" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="P36" t="n">
+        <v>42.49</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>9.57</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1767,6 +2397,24 @@
       <c r="I37" t="inlineStr"/>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
+      <c r="L37" t="n">
+        <v>35</v>
+      </c>
+      <c r="M37" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N37" t="n">
+        <v>9.02</v>
+      </c>
+      <c r="O37" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="P37" t="n">
+        <v>39.25</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>4.08</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1804,6 +2452,24 @@
       <c r="K38" t="n">
         <v>53.2</v>
       </c>
+      <c r="L38" t="n">
+        <v>36</v>
+      </c>
+      <c r="M38" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="N38" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="O38" t="n">
+        <v>7.44</v>
+      </c>
+      <c r="P38" t="n">
+        <v>35.63</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>7.19</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1845,6 +2511,24 @@
       <c r="K39" t="n">
         <v>69.69999999999999</v>
       </c>
+      <c r="L39" t="n">
+        <v>37</v>
+      </c>
+      <c r="M39" t="n">
+        <v>7.77</v>
+      </c>
+      <c r="N39" t="n">
+        <v>11.97</v>
+      </c>
+      <c r="O39" t="n">
+        <v>6.97</v>
+      </c>
+      <c r="P39" t="n">
+        <v>33.35</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>7.38</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1886,6 +2570,24 @@
       <c r="K40" t="n">
         <v>54</v>
       </c>
+      <c r="L40" t="n">
+        <v>38</v>
+      </c>
+      <c r="M40" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="N40" t="n">
+        <v>7.05</v>
+      </c>
+      <c r="O40" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="P40" t="n">
+        <v>16.65</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>5.55</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1926,6 +2628,24 @@
       </c>
       <c r="K41" t="n">
         <v>57.6</v>
+      </c>
+      <c r="L41" t="n">
+        <v>39</v>
+      </c>
+      <c r="M41" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="N41" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="O41" t="n">
+        <v>4.31</v>
+      </c>
+      <c r="P41" t="n">
+        <v>23.84</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>2.67</v>
       </c>
     </row>
     <row r="42">
@@ -1954,6 +2674,24 @@
       <c r="I42" t="inlineStr"/>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
+      <c r="L42" t="n">
+        <v>40</v>
+      </c>
+      <c r="M42" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="N42" t="n">
+        <v>33.63</v>
+      </c>
+      <c r="O42" t="n">
+        <v>18.78</v>
+      </c>
+      <c r="P42" t="n">
+        <v>48.11</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>42.11</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1994,6 +2732,24 @@
       </c>
       <c r="K43" t="n">
         <v>47.9</v>
+      </c>
+      <c r="L43" t="n">
+        <v>41</v>
+      </c>
+      <c r="M43" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="N43" t="n">
+        <v>12.43</v>
+      </c>
+      <c r="O43" t="n">
+        <v>6.76</v>
+      </c>
+      <c r="P43" t="n">
+        <v>37.4</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>7.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added bonds file from bloomberg Created visuals to explore this file
</commit_message>
<xml_diff>
--- a/Current_Model_Build.xlsx
+++ b/Current_Model_Build.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q43"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,30 +491,25 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>2023_WPR_ND_Risk_Exposure</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>2023_WPR_ND_Risk_Exposure</t>
+          <t>2023_WPR_ND_Risk_Vulnerability</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>2023_WPR_ND_Risk_Vulnerability</t>
+          <t>2023_WPR_ND_Risk_Susceptibility</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>2023_WPR_ND_Risk_Susceptibility</t>
+          <t>2023_WPR_ND_Lack_Adaptive_Capacities</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>2023_WPR_ND_Lack_Adaptive_Capacities</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>2023_WPR_ND_Lack_Coping_Capacities</t>
         </is>
@@ -547,21 +542,18 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
-        <v>0</v>
+        <v>2.29</v>
       </c>
       <c r="M2" t="n">
-        <v>2.29</v>
+        <v>16.95</v>
       </c>
       <c r="N2" t="n">
-        <v>16.95</v>
+        <v>11.51</v>
       </c>
       <c r="O2" t="n">
-        <v>11.51</v>
+        <v>37.51</v>
       </c>
       <c r="P2" t="n">
-        <v>37.51</v>
-      </c>
-      <c r="Q2" t="n">
         <v>11.28</v>
       </c>
     </row>
@@ -606,21 +598,18 @@
         <v>69.34999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>1</v>
+        <v>0.15</v>
       </c>
       <c r="M3" t="n">
-        <v>0.15</v>
+        <v>8.84</v>
       </c>
       <c r="N3" t="n">
-        <v>8.84</v>
+        <v>4.44</v>
       </c>
       <c r="O3" t="n">
-        <v>4.44</v>
+        <v>19.53</v>
       </c>
       <c r="P3" t="n">
-        <v>19.53</v>
-      </c>
-      <c r="Q3" t="n">
         <v>7.98</v>
       </c>
     </row>
@@ -659,21 +648,18 @@
         <v>24.3</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>0.05</v>
       </c>
       <c r="M4" t="n">
-        <v>0.05</v>
+        <v>11.14</v>
       </c>
       <c r="N4" t="n">
-        <v>11.14</v>
+        <v>6.49</v>
       </c>
       <c r="O4" t="n">
-        <v>6.49</v>
+        <v>36.57</v>
       </c>
       <c r="P4" t="n">
-        <v>36.57</v>
-      </c>
-      <c r="Q4" t="n">
         <v>5.83</v>
       </c>
     </row>
@@ -718,21 +704,18 @@
         <v>64.5</v>
       </c>
       <c r="L5" t="n">
-        <v>3</v>
+        <v>1.84</v>
       </c>
       <c r="M5" t="n">
-        <v>1.84</v>
+        <v>18.49</v>
       </c>
       <c r="N5" t="n">
-        <v>18.49</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="O5" t="n">
-        <v>8.029999999999999</v>
+        <v>28.91</v>
       </c>
       <c r="P5" t="n">
-        <v>28.91</v>
-      </c>
-      <c r="Q5" t="n">
         <v>27.21</v>
       </c>
     </row>
@@ -763,21 +746,18 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
-        <v>4</v>
+        <v>0.34</v>
       </c>
       <c r="M6" t="n">
-        <v>0.34</v>
+        <v>20.28</v>
       </c>
       <c r="N6" t="n">
-        <v>20.28</v>
+        <v>14.13</v>
       </c>
       <c r="O6" t="n">
-        <v>14.13</v>
+        <v>51.26</v>
       </c>
       <c r="P6" t="n">
-        <v>51.26</v>
-      </c>
-      <c r="Q6" t="n">
         <v>11.51</v>
       </c>
     </row>
@@ -818,21 +798,18 @@
         <v>25.55</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>0.3</v>
       </c>
       <c r="M7" t="n">
-        <v>0.3</v>
+        <v>19.15</v>
       </c>
       <c r="N7" t="n">
-        <v>19.15</v>
+        <v>17.48</v>
       </c>
       <c r="O7" t="n">
-        <v>17.48</v>
+        <v>46.46</v>
       </c>
       <c r="P7" t="n">
-        <v>46.46</v>
-      </c>
-      <c r="Q7" t="n">
         <v>8.65</v>
       </c>
     </row>
@@ -873,21 +850,18 @@
         <v>56.9</v>
       </c>
       <c r="L8" t="n">
-        <v>6</v>
+        <v>1.57</v>
       </c>
       <c r="M8" t="n">
-        <v>1.57</v>
+        <v>14.48</v>
       </c>
       <c r="N8" t="n">
-        <v>14.48</v>
+        <v>8.539999999999999</v>
       </c>
       <c r="O8" t="n">
-        <v>8.539999999999999</v>
+        <v>37.03</v>
       </c>
       <c r="P8" t="n">
-        <v>37.03</v>
-      </c>
-      <c r="Q8" t="n">
         <v>9.6</v>
       </c>
     </row>
@@ -928,21 +902,18 @@
         <v>36.3</v>
       </c>
       <c r="L9" t="n">
-        <v>7</v>
+        <v>1.02</v>
       </c>
       <c r="M9" t="n">
-        <v>1.02</v>
+        <v>12.43</v>
       </c>
       <c r="N9" t="n">
-        <v>12.43</v>
+        <v>7.26</v>
       </c>
       <c r="O9" t="n">
-        <v>7.26</v>
+        <v>35.48</v>
       </c>
       <c r="P9" t="n">
-        <v>35.48</v>
-      </c>
-      <c r="Q9" t="n">
         <v>7.45</v>
       </c>
     </row>
@@ -972,14 +943,11 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="n">
-        <v>8</v>
-      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1022,21 +990,18 @@
         <v>86.19999999999999</v>
       </c>
       <c r="L11" t="n">
-        <v>9</v>
+        <v>0.18</v>
       </c>
       <c r="M11" t="n">
-        <v>0.18</v>
+        <v>5.42</v>
       </c>
       <c r="N11" t="n">
-        <v>5.42</v>
+        <v>3.47</v>
       </c>
       <c r="O11" t="n">
-        <v>3.47</v>
+        <v>28.66</v>
       </c>
       <c r="P11" t="n">
-        <v>28.66</v>
-      </c>
-      <c r="Q11" t="n">
         <v>1.6</v>
       </c>
     </row>
@@ -1077,21 +1042,18 @@
         <v>83.69999999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>10</v>
+        <v>0.43</v>
       </c>
       <c r="M12" t="n">
-        <v>0.43</v>
+        <v>7.87</v>
       </c>
       <c r="N12" t="n">
-        <v>7.87</v>
+        <v>6.7</v>
       </c>
       <c r="O12" t="n">
-        <v>6.7</v>
+        <v>37.87</v>
       </c>
       <c r="P12" t="n">
-        <v>37.87</v>
-      </c>
-      <c r="Q12" t="n">
         <v>1.92</v>
       </c>
     </row>
@@ -1136,21 +1098,18 @@
         <v>89.3</v>
       </c>
       <c r="L13" t="n">
-        <v>11</v>
+        <v>0.49</v>
       </c>
       <c r="M13" t="n">
-        <v>0.49</v>
+        <v>4.2</v>
       </c>
       <c r="N13" t="n">
-        <v>4.2</v>
+        <v>5.71</v>
       </c>
       <c r="O13" t="n">
-        <v>5.71</v>
+        <v>26.53</v>
       </c>
       <c r="P13" t="n">
-        <v>26.53</v>
-      </c>
-      <c r="Q13" t="n">
         <v>0.49</v>
       </c>
     </row>
@@ -1195,21 +1154,18 @@
         <v>63.55</v>
       </c>
       <c r="L14" t="n">
-        <v>12</v>
+        <v>2.7</v>
       </c>
       <c r="M14" t="n">
-        <v>2.7</v>
+        <v>20.23</v>
       </c>
       <c r="N14" t="n">
-        <v>20.23</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="O14" t="n">
-        <v>8.460000000000001</v>
+        <v>33.29</v>
       </c>
       <c r="P14" t="n">
-        <v>33.29</v>
-      </c>
-      <c r="Q14" t="n">
         <v>29.38</v>
       </c>
     </row>
@@ -1254,21 +1210,18 @@
         <v>76.95</v>
       </c>
       <c r="L15" t="n">
-        <v>13</v>
+        <v>1.99</v>
       </c>
       <c r="M15" t="n">
-        <v>1.99</v>
+        <v>9.279999999999999</v>
       </c>
       <c r="N15" t="n">
-        <v>9.279999999999999</v>
+        <v>7.02</v>
       </c>
       <c r="O15" t="n">
-        <v>7.02</v>
+        <v>35.42</v>
       </c>
       <c r="P15" t="n">
-        <v>35.42</v>
-      </c>
-      <c r="Q15" t="n">
         <v>3.21</v>
       </c>
     </row>
@@ -1313,21 +1266,18 @@
         <v>52.24999999999999</v>
       </c>
       <c r="L16" t="n">
-        <v>14</v>
+        <v>8.25</v>
       </c>
       <c r="M16" t="n">
-        <v>8.25</v>
+        <v>8.93</v>
       </c>
       <c r="N16" t="n">
-        <v>8.93</v>
+        <v>8.82</v>
       </c>
       <c r="O16" t="n">
-        <v>8.82</v>
+        <v>9.98</v>
       </c>
       <c r="P16" t="n">
-        <v>9.98</v>
-      </c>
-      <c r="Q16" t="n">
         <v>8.09</v>
       </c>
     </row>
@@ -1368,21 +1318,18 @@
         <v>12.8</v>
       </c>
       <c r="L17" t="n">
-        <v>15</v>
+        <v>0.11</v>
       </c>
       <c r="M17" t="n">
-        <v>0.11</v>
+        <v>7.98</v>
       </c>
       <c r="N17" t="n">
-        <v>7.98</v>
+        <v>5.33</v>
       </c>
       <c r="O17" t="n">
-        <v>5.33</v>
+        <v>10.36</v>
       </c>
       <c r="P17" t="n">
-        <v>10.36</v>
-      </c>
-      <c r="Q17" t="n">
         <v>9.220000000000001</v>
       </c>
     </row>
@@ -1415,21 +1362,18 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="n">
-        <v>16</v>
+        <v>0.55</v>
       </c>
       <c r="M18" t="n">
-        <v>0.55</v>
+        <v>5.97</v>
       </c>
       <c r="N18" t="n">
-        <v>5.97</v>
+        <v>6.26</v>
       </c>
       <c r="O18" t="n">
-        <v>6.26</v>
+        <v>19.86</v>
       </c>
       <c r="P18" t="n">
-        <v>19.86</v>
-      </c>
-      <c r="Q18" t="n">
         <v>1.71</v>
       </c>
     </row>
@@ -1474,21 +1418,18 @@
         <v>50.4</v>
       </c>
       <c r="L19" t="n">
-        <v>17</v>
+        <v>1.45</v>
       </c>
       <c r="M19" t="n">
-        <v>1.45</v>
+        <v>7.3</v>
       </c>
       <c r="N19" t="n">
-        <v>7.3</v>
+        <v>4.59</v>
       </c>
       <c r="O19" t="n">
-        <v>4.59</v>
+        <v>24.76</v>
       </c>
       <c r="P19" t="n">
-        <v>24.76</v>
-      </c>
-      <c r="Q19" t="n">
         <v>3.43</v>
       </c>
     </row>
@@ -1533,21 +1474,18 @@
         <v>32.45</v>
       </c>
       <c r="L20" t="n">
-        <v>18</v>
+        <v>8.69</v>
       </c>
       <c r="M20" t="n">
-        <v>8.69</v>
+        <v>11.43</v>
       </c>
       <c r="N20" t="n">
-        <v>11.43</v>
+        <v>7.96</v>
       </c>
       <c r="O20" t="n">
-        <v>7.96</v>
+        <v>35.77</v>
       </c>
       <c r="P20" t="n">
-        <v>35.77</v>
-      </c>
-      <c r="Q20" t="n">
         <v>5.25</v>
       </c>
     </row>
@@ -1583,14 +1521,11 @@
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="n">
-        <v>19</v>
-      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
-      <c r="Q21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1618,14 +1553,11 @@
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
-      <c r="L22" t="n">
-        <v>20</v>
-      </c>
+      <c r="L22" t="inlineStr"/>
       <c r="M22" t="inlineStr"/>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1662,21 +1594,18 @@
         <v>56.9</v>
       </c>
       <c r="L23" t="n">
-        <v>21</v>
+        <v>0.79</v>
       </c>
       <c r="M23" t="n">
-        <v>0.79</v>
+        <v>9.49</v>
       </c>
       <c r="N23" t="n">
-        <v>9.49</v>
+        <v>9.289999999999999</v>
       </c>
       <c r="O23" t="n">
-        <v>9.289999999999999</v>
+        <v>40.13</v>
       </c>
       <c r="P23" t="n">
-        <v>40.13</v>
-      </c>
-      <c r="Q23" t="n">
         <v>2.29</v>
       </c>
     </row>
@@ -1715,21 +1644,18 @@
         <v>58.65</v>
       </c>
       <c r="L24" t="n">
-        <v>22</v>
+        <v>0.08</v>
       </c>
       <c r="M24" t="n">
-        <v>0.08</v>
+        <v>66.43000000000001</v>
       </c>
       <c r="N24" t="n">
-        <v>66.43000000000001</v>
+        <v>61.03</v>
       </c>
       <c r="O24" t="n">
-        <v>61.03</v>
+        <v>68.44</v>
       </c>
       <c r="P24" t="n">
-        <v>68.44</v>
-      </c>
-      <c r="Q24" t="n">
         <v>70.18000000000001</v>
       </c>
     </row>
@@ -1774,21 +1700,18 @@
         <v>57.6</v>
       </c>
       <c r="L25" t="n">
-        <v>23</v>
+        <v>0.06</v>
       </c>
       <c r="M25" t="n">
-        <v>0.06</v>
+        <v>6.81</v>
       </c>
       <c r="N25" t="n">
-        <v>6.81</v>
+        <v>5.36</v>
       </c>
       <c r="O25" t="n">
-        <v>5.36</v>
+        <v>10.22</v>
       </c>
       <c r="P25" t="n">
-        <v>10.22</v>
-      </c>
-      <c r="Q25" t="n">
         <v>5.76</v>
       </c>
     </row>
@@ -1827,21 +1750,18 @@
         <v>44.24999999999999</v>
       </c>
       <c r="L26" t="n">
-        <v>24</v>
+        <v>0.15</v>
       </c>
       <c r="M26" t="n">
-        <v>0.15</v>
+        <v>5.13</v>
       </c>
       <c r="N26" t="n">
-        <v>5.13</v>
+        <v>4.67</v>
       </c>
       <c r="O26" t="n">
-        <v>4.67</v>
+        <v>13.99</v>
       </c>
       <c r="P26" t="n">
-        <v>13.99</v>
-      </c>
-      <c r="Q26" t="n">
         <v>2.07</v>
       </c>
     </row>
@@ -1872,21 +1792,18 @@
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="n">
-        <v>25</v>
+        <v>0.1</v>
       </c>
       <c r="M27" t="n">
-        <v>0.1</v>
+        <v>17.72</v>
       </c>
       <c r="N27" t="n">
-        <v>17.72</v>
+        <v>11.78</v>
       </c>
       <c r="O27" t="n">
-        <v>11.78</v>
+        <v>48.54</v>
       </c>
       <c r="P27" t="n">
-        <v>48.54</v>
-      </c>
-      <c r="Q27" t="n">
         <v>9.73</v>
       </c>
     </row>
@@ -1917,21 +1834,18 @@
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="n">
-        <v>26</v>
+        <v>0.83</v>
       </c>
       <c r="M28" t="n">
-        <v>0.83</v>
+        <v>11.8</v>
       </c>
       <c r="N28" t="n">
-        <v>11.8</v>
+        <v>8.369999999999999</v>
       </c>
       <c r="O28" t="n">
-        <v>8.369999999999999</v>
+        <v>44.66</v>
       </c>
       <c r="P28" t="n">
-        <v>44.66</v>
-      </c>
-      <c r="Q28" t="n">
         <v>4.39</v>
       </c>
     </row>
@@ -1976,21 +1890,18 @@
         <v>93.34999999999999</v>
       </c>
       <c r="L29" t="n">
-        <v>27</v>
+        <v>2.2</v>
       </c>
       <c r="M29" t="n">
-        <v>2.2</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="N29" t="n">
-        <v>8.470000000000001</v>
+        <v>5.6</v>
       </c>
       <c r="O29" t="n">
-        <v>5.6</v>
+        <v>33.07</v>
       </c>
       <c r="P29" t="n">
-        <v>33.07</v>
-      </c>
-      <c r="Q29" t="n">
         <v>3.28</v>
       </c>
     </row>
@@ -2021,21 +1932,18 @@
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="n">
-        <v>28</v>
+        <v>0.33</v>
       </c>
       <c r="M30" t="n">
-        <v>0.33</v>
+        <v>5.12</v>
       </c>
       <c r="N30" t="n">
-        <v>5.12</v>
+        <v>8.07</v>
       </c>
       <c r="O30" t="n">
-        <v>8.07</v>
+        <v>7.43</v>
       </c>
       <c r="P30" t="n">
-        <v>7.43</v>
-      </c>
-      <c r="Q30" t="n">
         <v>2.24</v>
       </c>
     </row>
@@ -2080,21 +1988,18 @@
         <v>49.74999999999999</v>
       </c>
       <c r="L31" t="n">
-        <v>29</v>
+        <v>1.06</v>
       </c>
       <c r="M31" t="n">
-        <v>1.06</v>
+        <v>7.9</v>
       </c>
       <c r="N31" t="n">
-        <v>7.9</v>
+        <v>6.55</v>
       </c>
       <c r="O31" t="n">
-        <v>6.55</v>
+        <v>23.67</v>
       </c>
       <c r="P31" t="n">
-        <v>23.67</v>
-      </c>
-      <c r="Q31" t="n">
         <v>3.18</v>
       </c>
     </row>
@@ -2139,21 +2044,18 @@
         <v>31.65</v>
       </c>
       <c r="L32" t="n">
-        <v>30</v>
+        <v>1.73</v>
       </c>
       <c r="M32" t="n">
-        <v>1.73</v>
+        <v>10.28</v>
       </c>
       <c r="N32" t="n">
-        <v>10.28</v>
+        <v>5.2</v>
       </c>
       <c r="O32" t="n">
-        <v>5.2</v>
+        <v>40.15</v>
       </c>
       <c r="P32" t="n">
-        <v>40.15</v>
-      </c>
-      <c r="Q32" t="n">
         <v>5.21</v>
       </c>
     </row>
@@ -2198,21 +2100,18 @@
         <v>66.2</v>
       </c>
       <c r="L33" t="n">
-        <v>31</v>
+        <v>1.09</v>
       </c>
       <c r="M33" t="n">
-        <v>1.09</v>
+        <v>25.96</v>
       </c>
       <c r="N33" t="n">
-        <v>25.96</v>
+        <v>18.99</v>
       </c>
       <c r="O33" t="n">
-        <v>18.99</v>
+        <v>67.72</v>
       </c>
       <c r="P33" t="n">
-        <v>67.72</v>
-      </c>
-      <c r="Q33" t="n">
         <v>13.61</v>
       </c>
     </row>
@@ -2253,21 +2152,18 @@
         <v>58.89999999999999</v>
       </c>
       <c r="L34" t="n">
-        <v>32</v>
+        <v>0.71</v>
       </c>
       <c r="M34" t="n">
-        <v>0.71</v>
+        <v>15.6</v>
       </c>
       <c r="N34" t="n">
-        <v>15.6</v>
+        <v>9.25</v>
       </c>
       <c r="O34" t="n">
-        <v>9.25</v>
+        <v>47.28</v>
       </c>
       <c r="P34" t="n">
-        <v>47.28</v>
-      </c>
-      <c r="Q34" t="n">
         <v>8.68</v>
       </c>
     </row>
@@ -2308,21 +2204,18 @@
         <v>7.249999999999999</v>
       </c>
       <c r="L35" t="n">
-        <v>33</v>
+        <v>28.35</v>
       </c>
       <c r="M35" t="n">
-        <v>28.35</v>
+        <v>28.05</v>
       </c>
       <c r="N35" t="n">
-        <v>28.05</v>
+        <v>14.97</v>
       </c>
       <c r="O35" t="n">
-        <v>14.97</v>
+        <v>37.81</v>
       </c>
       <c r="P35" t="n">
-        <v>37.81</v>
-      </c>
-      <c r="Q35" t="n">
         <v>39</v>
       </c>
     </row>
@@ -2353,21 +2246,18 @@
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="n">
-        <v>34</v>
+        <v>0.17</v>
       </c>
       <c r="M36" t="n">
-        <v>0.17</v>
+        <v>17.92</v>
       </c>
       <c r="N36" t="n">
-        <v>17.92</v>
+        <v>14.15</v>
       </c>
       <c r="O36" t="n">
-        <v>14.15</v>
+        <v>42.49</v>
       </c>
       <c r="P36" t="n">
-        <v>42.49</v>
-      </c>
-      <c r="Q36" t="n">
         <v>9.57</v>
       </c>
     </row>
@@ -2398,21 +2288,18 @@
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="n">
-        <v>35</v>
+        <v>0.1</v>
       </c>
       <c r="M37" t="n">
-        <v>0.1</v>
+        <v>9.02</v>
       </c>
       <c r="N37" t="n">
-        <v>9.02</v>
+        <v>4.59</v>
       </c>
       <c r="O37" t="n">
-        <v>4.59</v>
+        <v>39.25</v>
       </c>
       <c r="P37" t="n">
-        <v>39.25</v>
-      </c>
-      <c r="Q37" t="n">
         <v>4.08</v>
       </c>
     </row>
@@ -2453,21 +2340,18 @@
         <v>53.2</v>
       </c>
       <c r="L38" t="n">
-        <v>36</v>
+        <v>0.31</v>
       </c>
       <c r="M38" t="n">
-        <v>0.31</v>
+        <v>12.4</v>
       </c>
       <c r="N38" t="n">
-        <v>12.4</v>
+        <v>7.44</v>
       </c>
       <c r="O38" t="n">
-        <v>7.44</v>
+        <v>35.63</v>
       </c>
       <c r="P38" t="n">
-        <v>35.63</v>
-      </c>
-      <c r="Q38" t="n">
         <v>7.19</v>
       </c>
     </row>
@@ -2512,21 +2396,18 @@
         <v>69.69999999999999</v>
       </c>
       <c r="L39" t="n">
-        <v>37</v>
+        <v>7.77</v>
       </c>
       <c r="M39" t="n">
-        <v>7.77</v>
+        <v>11.97</v>
       </c>
       <c r="N39" t="n">
-        <v>11.97</v>
+        <v>6.97</v>
       </c>
       <c r="O39" t="n">
-        <v>6.97</v>
+        <v>33.35</v>
       </c>
       <c r="P39" t="n">
-        <v>33.35</v>
-      </c>
-      <c r="Q39" t="n">
         <v>7.38</v>
       </c>
     </row>
@@ -2571,21 +2452,18 @@
         <v>54</v>
       </c>
       <c r="L40" t="n">
-        <v>38</v>
+        <v>1.05</v>
       </c>
       <c r="M40" t="n">
-        <v>1.05</v>
+        <v>7.05</v>
       </c>
       <c r="N40" t="n">
-        <v>7.05</v>
+        <v>3.8</v>
       </c>
       <c r="O40" t="n">
-        <v>3.8</v>
+        <v>16.65</v>
       </c>
       <c r="P40" t="n">
-        <v>16.65</v>
-      </c>
-      <c r="Q40" t="n">
         <v>5.55</v>
       </c>
     </row>
@@ -2630,21 +2508,18 @@
         <v>57.6</v>
       </c>
       <c r="L41" t="n">
-        <v>39</v>
+        <v>0.16</v>
       </c>
       <c r="M41" t="n">
-        <v>0.16</v>
+        <v>6.5</v>
       </c>
       <c r="N41" t="n">
-        <v>6.5</v>
+        <v>4.31</v>
       </c>
       <c r="O41" t="n">
-        <v>4.31</v>
+        <v>23.84</v>
       </c>
       <c r="P41" t="n">
-        <v>23.84</v>
-      </c>
-      <c r="Q41" t="n">
         <v>2.67</v>
       </c>
     </row>
@@ -2675,21 +2550,18 @@
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="n">
-        <v>40</v>
+        <v>0.48</v>
       </c>
       <c r="M42" t="n">
-        <v>0.48</v>
+        <v>33.63</v>
       </c>
       <c r="N42" t="n">
-        <v>33.63</v>
+        <v>18.78</v>
       </c>
       <c r="O42" t="n">
-        <v>18.78</v>
+        <v>48.11</v>
       </c>
       <c r="P42" t="n">
-        <v>48.11</v>
-      </c>
-      <c r="Q42" t="n">
         <v>42.11</v>
       </c>
     </row>
@@ -2734,21 +2606,18 @@
         <v>47.9</v>
       </c>
       <c r="L43" t="n">
-        <v>41</v>
+        <v>2.58</v>
       </c>
       <c r="M43" t="n">
-        <v>2.58</v>
+        <v>12.43</v>
       </c>
       <c r="N43" t="n">
-        <v>12.43</v>
+        <v>6.76</v>
       </c>
       <c r="O43" t="n">
-        <v>6.76</v>
+        <v>37.4</v>
       </c>
       <c r="P43" t="n">
-        <v>37.4</v>
-      </c>
-      <c r="Q43" t="n">
         <v>7.59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added score card, created more visualizations for  the presentation
</commit_message>
<xml_diff>
--- a/Current_Model_Build.xlsx
+++ b/Current_Model_Build.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,17 +516,12 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Nominal 2023 GDP (EUR Billions)</t>
+          <t>Labelled_Sustainable_Bonds_per_GDP</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Labelled Sustainable Bonds Issued per GDP</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Unlabelled Sustainable Bonds Issued per GDP</t>
+          <t>Unlabelled_Sustainable_Bonds_per_GDP</t>
         </is>
       </c>
     </row>
@@ -572,14 +567,11 @@
         <v>11.28</v>
       </c>
       <c r="Q2" t="n">
-        <v>21.8804</v>
+        <v>0</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -637,12 +629,9 @@
         <v>7.98</v>
       </c>
       <c r="Q3" t="n">
-        <v>499.8729</v>
+        <v>0.0245795483422591</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0245795483422591</v>
-      </c>
-      <c r="S3" t="n">
         <v>0.0329675889596315</v>
       </c>
     </row>
@@ -696,14 +685,11 @@
         <v>5.83</v>
       </c>
       <c r="Q4" t="n">
-        <v>65.4208</v>
+        <v>0</v>
       </c>
       <c r="R4" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -761,12 +747,9 @@
         <v>27.21</v>
       </c>
       <c r="Q5" t="n">
-        <v>596.13545</v>
+        <v>0.0309157844964049</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0309157844964049</v>
-      </c>
-      <c r="S5" t="n">
         <v>0.024776788847552</v>
       </c>
     </row>
@@ -812,12 +795,9 @@
         <v>11.51</v>
       </c>
       <c r="Q6" t="n">
-        <v>25.59775</v>
+        <v>0</v>
       </c>
       <c r="R6" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -873,12 +853,9 @@
         <v>8.65</v>
       </c>
       <c r="Q7" t="n">
-        <v>97.94405</v>
+        <v>0</v>
       </c>
       <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -934,12 +911,9 @@
         <v>9.6</v>
       </c>
       <c r="Q8" t="n">
-        <v>76.17574999999999</v>
+        <v>0.005244296175784</v>
       </c>
       <c r="R8" t="n">
-        <v>0.005244296175784</v>
-      </c>
-      <c r="S8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -996,7 +970,6 @@
       </c>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1030,12 +1003,9 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="n">
-        <v>318.48085</v>
+        <v>0.0045155238822032</v>
       </c>
       <c r="R10" t="n">
-        <v>0.0045155238822032</v>
-      </c>
-      <c r="S10" t="n">
         <v>0.0029464205311292</v>
       </c>
     </row>
@@ -1095,12 +1065,9 @@
         <v>1.6</v>
       </c>
       <c r="Q11" t="n">
-        <v>399.76</v>
+        <v>0.0162001009000484</v>
       </c>
       <c r="R11" t="n">
-        <v>0.0162001009000484</v>
-      </c>
-      <c r="S11" t="n">
         <v>0.06420129022045939</v>
       </c>
     </row>
@@ -1156,14 +1123,11 @@
         <v>1.92</v>
       </c>
       <c r="Q12" t="n">
-        <v>39.70905</v>
+        <v>0</v>
       </c>
       <c r="R12" t="n">
         <v>0</v>
       </c>
-      <c r="S12" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1221,12 +1185,9 @@
         <v>0.49</v>
       </c>
       <c r="Q13" t="n">
-        <v>290.40455</v>
+        <v>0.021201974327179</v>
       </c>
       <c r="R13" t="n">
-        <v>0.021201974327179</v>
-      </c>
-      <c r="S13" t="n">
         <v>0.0575590629061391</v>
       </c>
     </row>
@@ -1286,12 +1247,9 @@
         <v>29.38</v>
       </c>
       <c r="Q14" t="n">
-        <v>2896.5652</v>
+        <v>0.0214726359316581</v>
       </c>
       <c r="R14" t="n">
-        <v>0.0214726359316581</v>
-      </c>
-      <c r="S14" t="n">
         <v>0.0578502964252896</v>
       </c>
     </row>
@@ -1351,12 +1309,9 @@
         <v>3.21</v>
       </c>
       <c r="Q15" t="n">
-        <v>4208.3461</v>
+        <v>0.0117085281313705</v>
       </c>
       <c r="R15" t="n">
-        <v>0.0117085281313705</v>
-      </c>
-      <c r="S15" t="n">
         <v>0.0509871599412835</v>
       </c>
     </row>
@@ -1416,12 +1371,9 @@
         <v>8.09</v>
       </c>
       <c r="Q16" t="n">
-        <v>230.26575</v>
+        <v>0.0099620591422264</v>
       </c>
       <c r="R16" t="n">
-        <v>0.0099620591422264</v>
-      </c>
-      <c r="S16" t="n">
         <v>0.0006680373219732</v>
       </c>
     </row>
@@ -1477,12 +1429,9 @@
         <v>9.220000000000001</v>
       </c>
       <c r="Q17" t="n">
-        <v>193.63755</v>
+        <v>0.0246943212228768</v>
       </c>
       <c r="R17" t="n">
-        <v>0.0246943212228768</v>
-      </c>
-      <c r="S17" t="n">
         <v>0.02375134594897</v>
       </c>
     </row>
@@ -1530,12 +1479,9 @@
         <v>1.71</v>
       </c>
       <c r="Q18" t="n">
-        <v>29.0415</v>
+        <v>0.0539405463291679</v>
       </c>
       <c r="R18" t="n">
-        <v>0.0539405463291679</v>
-      </c>
-      <c r="S18" t="n">
         <v>0.0524176408498025</v>
       </c>
     </row>
@@ -1595,12 +1541,9 @@
         <v>3.43</v>
       </c>
       <c r="Q19" t="n">
-        <v>560.0905499999999</v>
+        <v>0.0246188260178055</v>
       </c>
       <c r="R19" t="n">
-        <v>0.0246188260178055</v>
-      </c>
-      <c r="S19" t="n">
         <v>0.0282178292653719</v>
       </c>
     </row>
@@ -1660,12 +1603,9 @@
         <v>5.25</v>
       </c>
       <c r="Q20" t="n">
-        <v>2076.7779</v>
+        <v>0.0120106819768944</v>
       </c>
       <c r="R20" t="n">
-        <v>0.0120106819768944</v>
-      </c>
-      <c r="S20" t="n">
         <v>0.0285602881840506</v>
       </c>
     </row>
@@ -1707,12 +1647,9 @@
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="n">
-        <v>6.62515</v>
+        <v>0.2283381399863999</v>
       </c>
       <c r="R21" t="n">
-        <v>0.2283381399863999</v>
-      </c>
-      <c r="S21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1748,12 +1685,9 @@
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="n">
-        <v>9.945550000000001</v>
+        <v>0</v>
       </c>
       <c r="R22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1807,12 +1741,9 @@
         <v>2.29</v>
       </c>
       <c r="Q23" t="n">
-        <v>44.3346</v>
+        <v>0.0029079233434606</v>
       </c>
       <c r="R23" t="n">
-        <v>0.0029079233434606</v>
-      </c>
-      <c r="S23" t="n">
         <v>0.0045477438682689</v>
       </c>
     </row>
@@ -1866,12 +1797,9 @@
         <v>70.18000000000001</v>
       </c>
       <c r="Q24" t="n">
-        <v>75.45565000000001</v>
+        <v>0.0066749203453017</v>
       </c>
       <c r="R24" t="n">
-        <v>0.0066749203453017</v>
-      </c>
-      <c r="S24" t="n">
         <v>0.0042941033575734</v>
       </c>
     </row>
@@ -1931,12 +1859,9 @@
         <v>5.76</v>
       </c>
       <c r="Q25" t="n">
-        <v>84.64024999999999</v>
+        <v>0.1416645543178077</v>
       </c>
       <c r="R25" t="n">
-        <v>0.1416645543178077</v>
-      </c>
-      <c r="S25" t="n">
         <v>0.1647783985557602</v>
       </c>
     </row>
@@ -1990,12 +1915,9 @@
         <v>2.07</v>
       </c>
       <c r="Q26" t="n">
-        <v>19.29545</v>
+        <v>0.0012876275861598</v>
       </c>
       <c r="R26" t="n">
-        <v>0.0012876275861598</v>
-      </c>
-      <c r="S26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2041,12 +1963,9 @@
         <v>9.73</v>
       </c>
       <c r="Q27" t="n">
-        <v>15.2</v>
+        <v>0</v>
       </c>
       <c r="R27" t="n">
-        <v>0</v>
-      </c>
-      <c r="S27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2092,14 +2011,11 @@
         <v>4.39</v>
       </c>
       <c r="Q28" t="n">
-        <v>6.7051</v>
+        <v>0</v>
       </c>
       <c r="R28" t="n">
         <v>0</v>
       </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2157,12 +2073,9 @@
         <v>3.28</v>
       </c>
       <c r="Q29" t="n">
-        <v>1038.1106</v>
+        <v>0.0488139515079503</v>
       </c>
       <c r="R29" t="n">
-        <v>0.0488139515079503</v>
-      </c>
-      <c r="S29" t="n">
         <v>0.1038073574729606</v>
       </c>
     </row>
@@ -2208,14 +2121,11 @@
         <v>2.24</v>
       </c>
       <c r="Q30" t="n">
-        <v>15.01095</v>
+        <v>0</v>
       </c>
       <c r="R30" t="n">
         <v>0</v>
       </c>
-      <c r="S30" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2273,12 +2183,9 @@
         <v>3.18</v>
       </c>
       <c r="Q31" t="n">
-        <v>519.4296000000001</v>
+        <v>0.0295927851678416</v>
       </c>
       <c r="R31" t="n">
-        <v>0.0295927851678416</v>
-      </c>
-      <c r="S31" t="n">
         <v>0.0766685380160143</v>
       </c>
     </row>
@@ -2338,12 +2245,9 @@
         <v>5.21</v>
       </c>
       <c r="Q32" t="n">
-        <v>800.0634</v>
+        <v>0.0016822142589665</v>
       </c>
       <c r="R32" t="n">
-        <v>0.0016822142589665</v>
-      </c>
-      <c r="S32" t="n">
         <v>0.0064251219592665</v>
       </c>
     </row>
@@ -2403,12 +2307,9 @@
         <v>13.61</v>
       </c>
       <c r="Q33" t="n">
-        <v>262.6104</v>
+        <v>0.004996442561761</v>
       </c>
       <c r="R33" t="n">
-        <v>0.004996442561761</v>
-      </c>
-      <c r="S33" t="n">
         <v>0.0245427051047459</v>
       </c>
     </row>
@@ -2464,12 +2365,9 @@
         <v>8.68</v>
       </c>
       <c r="Q34" t="n">
-        <v>332.8933</v>
+        <v>0.0065806567118448</v>
       </c>
       <c r="R34" t="n">
-        <v>0.0065806567118448</v>
-      </c>
-      <c r="S34" t="n">
         <v>0.0036853014270388</v>
       </c>
     </row>
@@ -2525,12 +2423,9 @@
         <v>39</v>
       </c>
       <c r="Q35" t="n">
-        <v>1769.3465</v>
+        <v>0.0004952184362180001</v>
       </c>
       <c r="R35" t="n">
-        <v>0.0004952184362180001</v>
-      </c>
-      <c r="S35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2576,12 +2471,9 @@
         <v>9.57</v>
       </c>
       <c r="Q36" t="n">
-        <v>71.26425</v>
+        <v>0.0151697440402572</v>
       </c>
       <c r="R36" t="n">
-        <v>0.0151697440402572</v>
-      </c>
-      <c r="S36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2627,12 +2519,9 @@
         <v>4.08</v>
       </c>
       <c r="Q37" t="n">
-        <v>126.3918</v>
+        <v>0.0039977576484559</v>
       </c>
       <c r="R37" t="n">
-        <v>0.0039977576484559</v>
-      </c>
-      <c r="S37" t="n">
         <v>0.0104108363132921</v>
       </c>
     </row>
@@ -2688,12 +2577,9 @@
         <v>7.19</v>
       </c>
       <c r="Q38" t="n">
-        <v>64.9743</v>
+        <v>0.0077629285747495</v>
       </c>
       <c r="R38" t="n">
-        <v>0.0077629285747495</v>
-      </c>
-      <c r="S38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2753,12 +2639,9 @@
         <v>7.38</v>
       </c>
       <c r="Q39" t="n">
-        <v>1502.9513</v>
+        <v>0.0161213056939449</v>
       </c>
       <c r="R39" t="n">
-        <v>0.0161213056939449</v>
-      </c>
-      <c r="S39" t="n">
         <v>0.0375768268903857</v>
       </c>
     </row>
@@ -2818,12 +2701,9 @@
         <v>5.55</v>
       </c>
       <c r="Q40" t="n">
-        <v>567.2545</v>
+        <v>0.0200204239021023</v>
       </c>
       <c r="R40" t="n">
-        <v>0.0200204239021023</v>
-      </c>
-      <c r="S40" t="n">
         <v>0.1028988360424584</v>
       </c>
     </row>
@@ -2883,12 +2763,9 @@
         <v>2.67</v>
       </c>
       <c r="Q41" t="n">
-        <v>860.3997999999999</v>
+        <v>0.0088299006743656</v>
       </c>
       <c r="R41" t="n">
-        <v>0.0088299006743656</v>
-      </c>
-      <c r="S41" t="n">
         <v>0.0085021998949229</v>
       </c>
     </row>
@@ -2934,12 +2811,9 @@
         <v>42.11</v>
       </c>
       <c r="Q42" t="n">
-        <v>164.74235</v>
+        <v>0.0046097664532357</v>
       </c>
       <c r="R42" t="n">
-        <v>0.0046097664532357</v>
-      </c>
-      <c r="S42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2999,12 +2873,9 @@
         <v>7.59</v>
       </c>
       <c r="Q43" t="n">
-        <v>3165.45605</v>
+        <v>0.0164649900888076</v>
       </c>
       <c r="R43" t="n">
-        <v>0.0164649900888076</v>
-      </c>
-      <c r="S43" t="n">
         <v>0.013492517092032</v>
       </c>
     </row>

</xml_diff>